<commit_message>
Update BCTR and BSoAIGtAP
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="BCTR" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="About" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="About" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="BCTR" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mi5ihDgixrKUk1H491dE8F35epCEg=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="LJgR9Cz38Cl6DQ4AMRtA9IGps69xyJgH90/JTrNzLQs="/>
     </ext>
   </extLst>
 </workbook>
@@ -18,6 +18,21 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>BCTR BAU Carbon Tax Rate</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>none needed</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>There is no carbon tax in Indonesia</t>
+  </si>
   <si>
     <t>Unit: $/metric ton CO2e</t>
   </si>
@@ -45,21 +60,6 @@
   <si>
     <t>geoengineering sector (uses industry sector rate)</t>
   </si>
-  <si>
-    <t>BCTR BAU Carbon Tax Rate</t>
-  </si>
-  <si>
-    <t>Source:</t>
-  </si>
-  <si>
-    <t>none needed</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>There is no carbon tax in Indonesia</t>
-  </si>
 </sst>
 </file>
 
@@ -73,13 +73,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -87,6 +80,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -339,7 +339,6 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <tabColor rgb="FF2F5496"/>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -347,919 +346,37 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.0"/>
-    <col customWidth="1" min="2" max="33" width="8.71"/>
+    <col customWidth="1" min="1" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <v>2019.0</v>
-      </c>
-      <c r="C1" s="2">
-        <v>2020.0</v>
-      </c>
-      <c r="D1" s="2">
-        <v>2021.0</v>
-      </c>
-      <c r="E1" s="2">
-        <v>2022.0</v>
-      </c>
-      <c r="F1" s="2">
-        <v>2023.0</v>
-      </c>
-      <c r="G1" s="2">
-        <v>2024.0</v>
-      </c>
-      <c r="H1" s="2">
-        <v>2025.0</v>
-      </c>
-      <c r="I1" s="2">
-        <v>2026.0</v>
-      </c>
-      <c r="J1" s="2">
-        <v>2027.0</v>
-      </c>
-      <c r="K1" s="2">
-        <v>2028.0</v>
-      </c>
-      <c r="L1" s="2">
-        <v>2029.0</v>
-      </c>
-      <c r="M1" s="2">
-        <v>2030.0</v>
-      </c>
-      <c r="N1" s="2">
-        <v>2031.0</v>
-      </c>
-      <c r="O1" s="2">
-        <v>2032.0</v>
-      </c>
-      <c r="P1" s="2">
-        <v>2033.0</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>2034.0</v>
-      </c>
-      <c r="R1" s="2">
-        <v>2035.0</v>
-      </c>
-      <c r="S1" s="2">
-        <v>2036.0</v>
-      </c>
-      <c r="T1" s="2">
-        <v>2037.0</v>
-      </c>
-      <c r="U1" s="2">
-        <v>2038.0</v>
-      </c>
-      <c r="V1" s="2">
-        <v>2039.0</v>
-      </c>
-      <c r="W1" s="2">
-        <v>2040.0</v>
-      </c>
-      <c r="X1" s="2">
-        <v>2041.0</v>
-      </c>
-      <c r="Y1" s="2">
-        <v>2042.0</v>
-      </c>
-      <c r="Z1" s="2">
-        <v>2043.0</v>
-      </c>
-      <c r="AA1" s="2">
-        <v>2044.0</v>
-      </c>
-      <c r="AB1" s="2">
-        <v>2045.0</v>
-      </c>
-      <c r="AC1" s="2">
-        <v>2046.0</v>
-      </c>
-      <c r="AD1" s="2">
-        <v>2047.0</v>
-      </c>
-      <c r="AE1" s="2">
-        <v>2048.0</v>
-      </c>
-      <c r="AF1" s="2">
-        <v>2049.0</v>
-      </c>
-      <c r="AG1" s="2">
-        <v>2050.0</v>
-      </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="14.25" customHeight="1"/>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="O2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="P2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="R2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="S2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="T2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="U2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="V2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="W2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="X2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AE2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AG2" s="3">
-        <v>0.0</v>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="O3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="P3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="R3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="S3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="T3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="U3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="V3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="W3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="X3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Y3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Z3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AA3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AC3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AE3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AF3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AG3" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="R4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="S4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="T4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="U4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="V4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="W4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="X4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AC4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AE4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AF4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AG4" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="P5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="R5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="T5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="V5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="W5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="X5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AB5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AC5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AD5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AE5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AF5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AG5" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="R6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="T6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="X6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AC6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AD6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AE6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AF6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AG6" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="N7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="O7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="P7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="R7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="S7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="T7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="U7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="V7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="W7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="X7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Y7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="Z7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AD7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AE7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AF7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AG7" s="3">
-        <v>0.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="R8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="S8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="T8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="U8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="V8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="W8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="X8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="Y8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="Z8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AA8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AB8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AC8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AD8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AE8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AF8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AG8" s="4">
-        <v>0.0</v>
+      <c r="A8" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="O9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="P9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="R9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="S9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="T9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="U9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="V9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="W9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="X9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="Y9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="Z9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AA9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AB9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AC9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AD9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AE9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AF9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AG9" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
+    <row r="9" ht="14.25" customHeight="1"/>
     <row r="10" ht="14.25" customHeight="1"/>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1"/>
@@ -2262,6 +1379,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FF2F5496"/>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -2269,37 +1387,919 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="48.0"/>
+    <col customWidth="1" min="2" max="33" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2019.0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2020.0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2023.0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2024.0</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025.0</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2026.0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2027.0</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2028.0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2029.0</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2030.0</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2031.0</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2032.0</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2033.0</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2034.0</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2035.0</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2036.0</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2037.0</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2038.0</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2039.0</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2040.0</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2041.0</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2042.0</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2043.0</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2044.0</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2045.0</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2046.0</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2047.0</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2048.0</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>2049.0</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>2050.0</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>0.0</v>
+      </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
+      <c r="B6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>0.0</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="W7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="T8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="V8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AC8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="V9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="W9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AB9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AC9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AD9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AE9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AF9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AG9" s="4">
+        <v>0.0</v>
+      </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1"/>
     <row r="10" ht="14.25" customHeight="1"/>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1"/>

</xml_diff>